<commit_message>
docs: add mais testes na planilha de teste - SERVICES 1
</commit_message>
<xml_diff>
--- a/documentação/planilha-de-teste/planilha-de-teste.xlsx
+++ b/documentação/planilha-de-teste/planilha-de-teste.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="44">
   <si>
     <t>CENÁRIO</t>
   </si>
@@ -176,6 +176,48 @@
   </si>
   <si>
     <t>Dado que eu esteja atualizando usuário associado por ID. Quando eu atualizar e não encontrar por ID. Então deve lançar exceção dizendo que não foi possível encontrar por ID.</t>
+  </si>
+  <si>
+    <t>TESTES API USERS - SERVICES</t>
+  </si>
+  <si>
+    <t>001 - Find All Users</t>
+  </si>
+  <si>
+    <t>CT001-001 - Encontrar todos os usuários deve retornar uma lista Pageable</t>
+  </si>
+  <si>
+    <t>Dado que eu esteja buscando todos os usuários. Quando eu buscar por todos os usuários. Então deve retornar uma lista de usuário Pageable, com tamanho da lista e ordem.</t>
+  </si>
+  <si>
+    <t>002 - Find Users By Username</t>
+  </si>
+  <si>
+    <t>CT002-001 - Encontrar usuários por username deve retornar uma lista de usuários relacionados a aquele nome, mesmo que passe apenas alguns caracteres, por exemplo: "mat"</t>
+  </si>
+  <si>
+    <t>Dado que eu esteja buscando usuário pelo username. Quando eu buscar por username. Então deve retornar uma lista de usuário relacionado a aquele username, com tamanho da página (lista)</t>
+  </si>
+  <si>
+    <t>003 - Find User By Id</t>
+  </si>
+  <si>
+    <t>CT003-001 - Encontrar usuário por ID deve retornar usuário relacionado a aquele ID</t>
+  </si>
+  <si>
+    <t>Dado que eu esteja buscando usuário por ID. Quando eu buscar por ID. Então deve retornar o usuário relacionado a aquele ID.</t>
+  </si>
+  <si>
+    <t>CT003-002 - Caso não encontrar usuário por ID, então deve retonar exceção "No records found for this id!"</t>
+  </si>
+  <si>
+    <t>Dado que eu esteja buscando usuário por ID. Quando eu buscar por ID. Então deve lançar exceção se não encontrar usuário por ID.</t>
+  </si>
+  <si>
+    <t>CT003-002 - Encontrar usuário por ID deve retornar link HATEOAS.</t>
+  </si>
+  <si>
+    <t>Dado que eu esteja buscando usuário por ID. Quando eu buscar por ID. Então deve retornar o usuário e o link HATEOAS.</t>
   </si>
 </sst>
 </file>
@@ -248,7 +290,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="6">
+  <borders count="10">
     <border>
       <left/>
       <right/>
@@ -321,11 +363,55 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -336,18 +422,32 @@
     <xf numFmtId="0" fontId="1" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -357,28 +457,26 @@
     <xf numFmtId="0" fontId="1" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -660,10 +758,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:H101"/>
+  <dimension ref="B2:H102"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="H51" sqref="H51"/>
+    <sheetView tabSelected="1" topLeftCell="A59" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2:E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -676,454 +774,679 @@
     <col min="8" max="8" width="17.81640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:8" ht="18.5" x14ac:dyDescent="0.45">
-      <c r="B2" s="6" t="s">
+    <row r="2" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="B2" s="17" t="s">
         <v>10</v>
       </c>
-      <c r="C2" s="6"/>
-      <c r="D2" s="6"/>
-      <c r="E2" s="6"/>
-      <c r="G2" s="8" t="s">
+      <c r="C2" s="17"/>
+      <c r="D2" s="17"/>
+      <c r="E2" s="17"/>
+    </row>
+    <row r="3" spans="2:8" ht="18.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B3" s="17"/>
+      <c r="C3" s="17"/>
+      <c r="D3" s="17"/>
+      <c r="E3" s="17"/>
+      <c r="G3" s="14" t="s">
         <v>3</v>
       </c>
-      <c r="H2" s="8"/>
-    </row>
-    <row r="3" spans="2:8" x14ac:dyDescent="0.35">
-      <c r="B3" s="1" t="s">
+      <c r="H3" s="14"/>
+    </row>
+    <row r="4" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="B4" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="1" t="s">
+      <c r="C4" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="D3" s="1" t="s">
+      <c r="D4" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="E3" s="1" t="s">
+      <c r="E4" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="G3" s="9" t="s">
+      <c r="G4" s="15" t="s">
         <v>4</v>
       </c>
-      <c r="H3" s="10"/>
-    </row>
-    <row r="4" spans="2:8" x14ac:dyDescent="0.35">
-      <c r="B4" s="15" t="s">
+      <c r="H4" s="16"/>
+    </row>
+    <row r="5" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="B5" s="12" t="s">
         <v>11</v>
       </c>
-      <c r="C4" s="5" t="s">
+      <c r="C5" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="D4" s="5" t="s">
+      <c r="D5" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="E4" s="13"/>
-      <c r="F4" s="11"/>
-      <c r="G4" s="2" t="s">
+      <c r="E5" s="7"/>
+      <c r="F5" s="4"/>
+      <c r="G5" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="H4" s="3"/>
-    </row>
-    <row r="5" spans="2:8" x14ac:dyDescent="0.35">
-      <c r="B5" s="16"/>
-      <c r="C5" s="5"/>
-      <c r="D5" s="5"/>
-      <c r="E5" s="13"/>
-      <c r="G5" s="2" t="s">
+      <c r="H5" s="3"/>
+    </row>
+    <row r="6" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="B6" s="13"/>
+      <c r="C6" s="8"/>
+      <c r="D6" s="8"/>
+      <c r="E6" s="7"/>
+      <c r="G6" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="H5" s="3"/>
-    </row>
-    <row r="6" spans="2:8" x14ac:dyDescent="0.35">
-      <c r="B6" s="16"/>
-      <c r="C6" s="5"/>
-      <c r="D6" s="5"/>
-      <c r="E6" s="13"/>
-    </row>
-    <row r="7" spans="2:8" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B7" s="16"/>
-      <c r="C7" s="5" t="s">
+      <c r="H6" s="3"/>
+    </row>
+    <row r="7" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="B7" s="13"/>
+      <c r="C7" s="8"/>
+      <c r="D7" s="8"/>
+      <c r="E7" s="7"/>
+    </row>
+    <row r="8" spans="2:8" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B8" s="13"/>
+      <c r="C8" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="D7" s="5" t="s">
+      <c r="D8" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="E7" s="13"/>
-      <c r="G7" s="12" t="s">
+      <c r="E8" s="7"/>
+      <c r="G8" s="14" t="s">
         <v>7</v>
       </c>
-      <c r="H7" s="12"/>
-    </row>
-    <row r="8" spans="2:8" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B8" s="16"/>
-      <c r="C8" s="5"/>
-      <c r="D8" s="5"/>
-      <c r="E8" s="13"/>
-      <c r="G8" s="17" t="s">
+      <c r="H8" s="14"/>
+    </row>
+    <row r="9" spans="2:8" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B9" s="13"/>
+      <c r="C9" s="8"/>
+      <c r="D9" s="8"/>
+      <c r="E9" s="7"/>
+      <c r="G9" s="19" t="s">
         <v>8</v>
       </c>
-      <c r="H8" s="17"/>
-    </row>
-    <row r="9" spans="2:8" x14ac:dyDescent="0.35">
-      <c r="B9" s="16"/>
-      <c r="C9" s="5"/>
-      <c r="D9" s="5"/>
-      <c r="E9" s="13"/>
-      <c r="G9" s="17"/>
-      <c r="H9" s="17"/>
+      <c r="H9" s="19"/>
     </row>
     <row r="10" spans="2:8" x14ac:dyDescent="0.35">
-      <c r="B10" s="16"/>
-      <c r="C10" s="5"/>
-      <c r="D10" s="5"/>
-      <c r="E10" s="13"/>
-      <c r="G10" s="17"/>
-      <c r="H10" s="17"/>
-    </row>
-    <row r="11" spans="2:8" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B11" s="16"/>
-      <c r="C11" s="5"/>
-      <c r="D11" s="5"/>
-      <c r="E11" s="13"/>
-      <c r="G11" s="17" t="s">
+      <c r="B10" s="13"/>
+      <c r="C10" s="8"/>
+      <c r="D10" s="8"/>
+      <c r="E10" s="7"/>
+      <c r="G10" s="19"/>
+      <c r="H10" s="19"/>
+    </row>
+    <row r="11" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="B11" s="13"/>
+      <c r="C11" s="8"/>
+      <c r="D11" s="8"/>
+      <c r="E11" s="7"/>
+      <c r="G11" s="19"/>
+      <c r="H11" s="19"/>
+    </row>
+    <row r="12" spans="2:8" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B12" s="13"/>
+      <c r="C12" s="8"/>
+      <c r="D12" s="8"/>
+      <c r="E12" s="7"/>
+      <c r="G12" s="20" t="s">
         <v>9</v>
       </c>
-      <c r="H11" s="17"/>
-    </row>
-    <row r="12" spans="2:8" ht="18" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B12" s="16"/>
-      <c r="C12" s="5"/>
-      <c r="D12" s="5"/>
-      <c r="E12" s="13"/>
-      <c r="G12" s="17"/>
-      <c r="H12" s="17"/>
-    </row>
-    <row r="13" spans="2:8" ht="14.5" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B13" s="16"/>
-      <c r="C13" s="14"/>
-      <c r="D13" s="14"/>
-      <c r="E13" s="14"/>
-      <c r="G13" s="17"/>
-      <c r="H13" s="17"/>
+      <c r="H12" s="21"/>
+    </row>
+    <row r="13" spans="2:8" ht="18" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B13" s="13"/>
+      <c r="C13" s="8"/>
+      <c r="D13" s="8"/>
+      <c r="E13" s="7"/>
+      <c r="G13" s="22"/>
+      <c r="H13" s="23"/>
     </row>
     <row r="14" spans="2:8" ht="14.5" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B14" s="16"/>
-      <c r="C14" s="14"/>
-      <c r="D14" s="14"/>
-      <c r="E14" s="14"/>
-      <c r="G14" s="17"/>
-      <c r="H14" s="17"/>
+      <c r="B14" s="13"/>
+      <c r="C14" s="5"/>
+      <c r="D14" s="5"/>
+      <c r="E14" s="5"/>
+      <c r="G14" s="18"/>
+      <c r="H14" s="18"/>
     </row>
     <row r="15" spans="2:8" ht="14.5" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B15" s="16"/>
-      <c r="C15" s="14"/>
-      <c r="D15" s="14"/>
-      <c r="E15" s="14"/>
-      <c r="G15" s="17"/>
-      <c r="H15" s="17"/>
+      <c r="B15" s="13"/>
+      <c r="C15" s="5"/>
+      <c r="D15" s="5"/>
+      <c r="E15" s="5"/>
+      <c r="G15" s="18"/>
+      <c r="H15" s="18"/>
     </row>
     <row r="16" spans="2:8" ht="14.5" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B16" s="16"/>
-      <c r="C16" s="14"/>
-      <c r="D16" s="14"/>
-      <c r="E16" s="14"/>
-      <c r="G16" s="17"/>
-      <c r="H16" s="17"/>
+      <c r="B16" s="13"/>
+      <c r="C16" s="5"/>
+      <c r="D16" s="5"/>
+      <c r="E16" s="5"/>
+      <c r="G16" s="18"/>
+      <c r="H16" s="18"/>
     </row>
     <row r="17" spans="2:8" ht="14.5" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B17" s="16"/>
-      <c r="C17" s="14"/>
-      <c r="D17" s="14"/>
-      <c r="E17" s="14"/>
-      <c r="G17" s="17"/>
-      <c r="H17" s="17"/>
-    </row>
-    <row r="18" spans="2:8" ht="14.5" hidden="1" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B18" s="16"/>
-      <c r="C18" s="18"/>
-      <c r="D18" s="18"/>
-      <c r="E18" s="18"/>
-      <c r="G18" s="17"/>
-      <c r="H18" s="17"/>
-    </row>
-    <row r="19" spans="2:8" ht="43.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B19" s="7" t="s">
+      <c r="B17" s="13"/>
+      <c r="C17" s="5"/>
+      <c r="D17" s="5"/>
+      <c r="E17" s="5"/>
+      <c r="G17" s="18"/>
+      <c r="H17" s="18"/>
+    </row>
+    <row r="18" spans="2:8" ht="14.5" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B18" s="13"/>
+      <c r="C18" s="5"/>
+      <c r="D18" s="5"/>
+      <c r="E18" s="5"/>
+      <c r="G18" s="18"/>
+      <c r="H18" s="18"/>
+    </row>
+    <row r="19" spans="2:8" ht="14.5" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B19" s="13"/>
+      <c r="C19" s="6"/>
+      <c r="D19" s="6"/>
+      <c r="E19" s="6"/>
+      <c r="G19" s="18"/>
+      <c r="H19" s="18"/>
+    </row>
+    <row r="20" spans="2:8" ht="43.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B20" s="11" t="s">
         <v>16</v>
       </c>
-      <c r="C19" s="5" t="s">
+      <c r="C20" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="D19" s="5" t="s">
+      <c r="D20" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="E19" s="19"/>
-      <c r="G19" s="17"/>
-      <c r="H19" s="17"/>
-    </row>
-    <row r="20" spans="2:8" x14ac:dyDescent="0.35">
-      <c r="B20" s="7"/>
-      <c r="C20" s="5"/>
-      <c r="D20" s="5"/>
-      <c r="E20" s="19"/>
-      <c r="G20" s="17"/>
-      <c r="H20" s="17"/>
+      <c r="E20" s="10"/>
     </row>
     <row r="21" spans="2:8" x14ac:dyDescent="0.35">
-      <c r="B21" s="7"/>
-      <c r="C21" s="5"/>
-      <c r="D21" s="5"/>
-      <c r="E21" s="19"/>
+      <c r="B21" s="11"/>
+      <c r="C21" s="8"/>
+      <c r="D21" s="8"/>
+      <c r="E21" s="10"/>
     </row>
     <row r="22" spans="2:8" x14ac:dyDescent="0.35">
-      <c r="B22" s="7"/>
-      <c r="C22" s="5"/>
-      <c r="D22" s="5"/>
-      <c r="E22" s="19"/>
+      <c r="B22" s="11"/>
+      <c r="C22" s="8"/>
+      <c r="D22" s="8"/>
+      <c r="E22" s="10"/>
     </row>
     <row r="23" spans="2:8" x14ac:dyDescent="0.35">
-      <c r="B23" s="7"/>
-      <c r="C23" s="5"/>
-      <c r="D23" s="5"/>
-      <c r="E23" s="19"/>
+      <c r="B23" s="11"/>
+      <c r="C23" s="8"/>
+      <c r="D23" s="8"/>
+      <c r="E23" s="10"/>
     </row>
     <row r="24" spans="2:8" x14ac:dyDescent="0.35">
-      <c r="B24" s="7"/>
-      <c r="C24" s="5"/>
-      <c r="D24" s="5"/>
-      <c r="E24" s="19"/>
+      <c r="B24" s="11"/>
+      <c r="C24" s="8"/>
+      <c r="D24" s="8"/>
+      <c r="E24" s="10"/>
     </row>
     <row r="25" spans="2:8" x14ac:dyDescent="0.35">
-      <c r="B25" s="7"/>
-      <c r="C25" s="5" t="s">
+      <c r="B25" s="11"/>
+      <c r="C25" s="8"/>
+      <c r="D25" s="8"/>
+      <c r="E25" s="10"/>
+    </row>
+    <row r="26" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="B26" s="11"/>
+      <c r="C26" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="D25" s="5" t="s">
+      <c r="D26" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="E25" s="13"/>
-    </row>
-    <row r="26" spans="2:8" x14ac:dyDescent="0.35">
-      <c r="B26" s="7"/>
-      <c r="C26" s="5"/>
-      <c r="D26" s="5"/>
-      <c r="E26" s="13"/>
+      <c r="E26" s="7"/>
     </row>
     <row r="27" spans="2:8" x14ac:dyDescent="0.35">
-      <c r="B27" s="7"/>
-      <c r="C27" s="5"/>
-      <c r="D27" s="5"/>
-      <c r="E27" s="13"/>
+      <c r="B27" s="11"/>
+      <c r="C27" s="8"/>
+      <c r="D27" s="8"/>
+      <c r="E27" s="7"/>
     </row>
     <row r="28" spans="2:8" x14ac:dyDescent="0.35">
-      <c r="B28" s="7"/>
-      <c r="C28" s="5"/>
-      <c r="D28" s="5"/>
-      <c r="E28" s="13"/>
+      <c r="B28" s="11"/>
+      <c r="C28" s="8"/>
+      <c r="D28" s="8"/>
+      <c r="E28" s="7"/>
     </row>
     <row r="29" spans="2:8" x14ac:dyDescent="0.35">
-      <c r="B29" s="7"/>
-      <c r="C29" s="5"/>
-      <c r="D29" s="5"/>
-      <c r="E29" s="13"/>
+      <c r="B29" s="11"/>
+      <c r="C29" s="8"/>
+      <c r="D29" s="8"/>
+      <c r="E29" s="7"/>
     </row>
     <row r="30" spans="2:8" x14ac:dyDescent="0.35">
-      <c r="B30" s="7"/>
-      <c r="C30" s="5"/>
-      <c r="D30" s="5"/>
-      <c r="E30" s="13"/>
+      <c r="B30" s="11"/>
+      <c r="C30" s="8"/>
+      <c r="D30" s="8"/>
+      <c r="E30" s="7"/>
     </row>
     <row r="31" spans="2:8" x14ac:dyDescent="0.35">
-      <c r="B31" s="4" t="s">
+      <c r="B31" s="11"/>
+      <c r="C31" s="8"/>
+      <c r="D31" s="8"/>
+      <c r="E31" s="7"/>
+    </row>
+    <row r="32" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="B32" s="9" t="s">
         <v>21</v>
       </c>
-      <c r="C31" s="5" t="s">
+      <c r="C32" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="D31" s="5" t="s">
+      <c r="D32" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="E31" s="13"/>
-    </row>
-    <row r="32" spans="2:8" x14ac:dyDescent="0.35">
-      <c r="B32" s="4"/>
-      <c r="C32" s="5"/>
-      <c r="D32" s="5"/>
-      <c r="E32" s="13"/>
+      <c r="E32" s="7"/>
     </row>
     <row r="33" spans="2:5" x14ac:dyDescent="0.35">
-      <c r="B33" s="4"/>
-      <c r="C33" s="5"/>
-      <c r="D33" s="5"/>
-      <c r="E33" s="13"/>
+      <c r="B33" s="9"/>
+      <c r="C33" s="8"/>
+      <c r="D33" s="8"/>
+      <c r="E33" s="7"/>
     </row>
     <row r="34" spans="2:5" x14ac:dyDescent="0.35">
-      <c r="B34" s="4"/>
-      <c r="C34" s="5"/>
-      <c r="D34" s="5"/>
-      <c r="E34" s="13"/>
+      <c r="B34" s="9"/>
+      <c r="C34" s="8"/>
+      <c r="D34" s="8"/>
+      <c r="E34" s="7"/>
     </row>
     <row r="35" spans="2:5" x14ac:dyDescent="0.35">
-      <c r="B35" s="4"/>
-      <c r="C35" s="5"/>
-      <c r="D35" s="5"/>
-      <c r="E35" s="13"/>
+      <c r="B35" s="9"/>
+      <c r="C35" s="8"/>
+      <c r="D35" s="8"/>
+      <c r="E35" s="7"/>
     </row>
     <row r="36" spans="2:5" x14ac:dyDescent="0.35">
-      <c r="B36" s="4"/>
-      <c r="C36" s="5"/>
-      <c r="D36" s="5"/>
-      <c r="E36" s="13"/>
+      <c r="B36" s="9"/>
+      <c r="C36" s="8"/>
+      <c r="D36" s="8"/>
+      <c r="E36" s="7"/>
     </row>
     <row r="37" spans="2:5" x14ac:dyDescent="0.35">
-      <c r="B37" s="4"/>
-      <c r="C37" s="5" t="s">
+      <c r="B37" s="9"/>
+      <c r="C37" s="8"/>
+      <c r="D37" s="8"/>
+      <c r="E37" s="7"/>
+    </row>
+    <row r="38" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B38" s="9"/>
+      <c r="C38" s="8" t="s">
         <v>24</v>
       </c>
-      <c r="D37" s="5" t="s">
+      <c r="D38" s="8" t="s">
         <v>25</v>
       </c>
-      <c r="E37" s="13"/>
-    </row>
-    <row r="38" spans="2:5" x14ac:dyDescent="0.35">
-      <c r="B38" s="4"/>
-      <c r="C38" s="5"/>
-      <c r="D38" s="5"/>
-      <c r="E38" s="13"/>
+      <c r="E38" s="7"/>
     </row>
     <row r="39" spans="2:5" x14ac:dyDescent="0.35">
-      <c r="B39" s="4"/>
-      <c r="C39" s="5"/>
-      <c r="D39" s="5"/>
-      <c r="E39" s="13"/>
+      <c r="B39" s="9"/>
+      <c r="C39" s="8"/>
+      <c r="D39" s="8"/>
+      <c r="E39" s="7"/>
     </row>
     <row r="40" spans="2:5" x14ac:dyDescent="0.35">
-      <c r="B40" s="4"/>
-      <c r="C40" s="5"/>
-      <c r="D40" s="5"/>
-      <c r="E40" s="13"/>
+      <c r="B40" s="9"/>
+      <c r="C40" s="8"/>
+      <c r="D40" s="8"/>
+      <c r="E40" s="7"/>
     </row>
     <row r="41" spans="2:5" x14ac:dyDescent="0.35">
-      <c r="B41" s="4"/>
-      <c r="C41" s="5"/>
-      <c r="D41" s="5"/>
-      <c r="E41" s="13"/>
+      <c r="B41" s="9"/>
+      <c r="C41" s="8"/>
+      <c r="D41" s="8"/>
+      <c r="E41" s="7"/>
     </row>
     <row r="42" spans="2:5" x14ac:dyDescent="0.35">
-      <c r="B42" s="4"/>
-      <c r="C42" s="5" t="s">
+      <c r="B42" s="9"/>
+      <c r="C42" s="8"/>
+      <c r="D42" s="8"/>
+      <c r="E42" s="7"/>
+    </row>
+    <row r="43" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B43" s="9"/>
+      <c r="C43" s="8" t="s">
         <v>26</v>
       </c>
-      <c r="D42" s="5" t="s">
+      <c r="D43" s="8" t="s">
         <v>27</v>
       </c>
-      <c r="E42" s="13"/>
-    </row>
-    <row r="43" spans="2:5" x14ac:dyDescent="0.35">
-      <c r="B43" s="4"/>
-      <c r="C43" s="5"/>
-      <c r="D43" s="5"/>
-      <c r="E43" s="13"/>
+      <c r="E43" s="7"/>
     </row>
     <row r="44" spans="2:5" x14ac:dyDescent="0.35">
-      <c r="B44" s="4"/>
-      <c r="C44" s="5"/>
-      <c r="D44" s="5"/>
-      <c r="E44" s="13"/>
+      <c r="B44" s="9"/>
+      <c r="C44" s="8"/>
+      <c r="D44" s="8"/>
+      <c r="E44" s="7"/>
     </row>
     <row r="45" spans="2:5" x14ac:dyDescent="0.35">
-      <c r="B45" s="4"/>
-      <c r="C45" s="5"/>
-      <c r="D45" s="5"/>
-      <c r="E45" s="13"/>
+      <c r="B45" s="9"/>
+      <c r="C45" s="8"/>
+      <c r="D45" s="8"/>
+      <c r="E45" s="7"/>
     </row>
     <row r="46" spans="2:5" x14ac:dyDescent="0.35">
-      <c r="B46" s="4"/>
-      <c r="C46" s="5"/>
-      <c r="D46" s="5"/>
-      <c r="E46" s="13"/>
+      <c r="B46" s="9"/>
+      <c r="C46" s="8"/>
+      <c r="D46" s="8"/>
+      <c r="E46" s="7"/>
     </row>
     <row r="47" spans="2:5" x14ac:dyDescent="0.35">
-      <c r="B47" s="4"/>
-      <c r="C47" s="5"/>
-      <c r="D47" s="5"/>
-      <c r="E47" s="13"/>
+      <c r="B47" s="9"/>
+      <c r="C47" s="8"/>
+      <c r="D47" s="8"/>
+      <c r="E47" s="7"/>
     </row>
     <row r="48" spans="2:5" x14ac:dyDescent="0.35">
-      <c r="B48" s="4"/>
-      <c r="C48" s="5" t="s">
+      <c r="B48" s="9"/>
+      <c r="C48" s="8"/>
+      <c r="D48" s="8"/>
+      <c r="E48" s="7"/>
+    </row>
+    <row r="49" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B49" s="9"/>
+      <c r="C49" s="8" t="s">
         <v>28</v>
       </c>
-      <c r="D48" s="5" t="s">
+      <c r="D49" s="8" t="s">
         <v>29</v>
       </c>
-      <c r="E48" s="13"/>
-    </row>
-    <row r="49" spans="2:5" x14ac:dyDescent="0.35">
-      <c r="B49" s="4"/>
-      <c r="C49" s="5"/>
-      <c r="D49" s="5"/>
-      <c r="E49" s="13"/>
+      <c r="E49" s="7"/>
     </row>
     <row r="50" spans="2:5" x14ac:dyDescent="0.35">
-      <c r="B50" s="4"/>
-      <c r="C50" s="5"/>
-      <c r="D50" s="5"/>
-      <c r="E50" s="13"/>
+      <c r="B50" s="9"/>
+      <c r="C50" s="8"/>
+      <c r="D50" s="8"/>
+      <c r="E50" s="7"/>
     </row>
     <row r="51" spans="2:5" x14ac:dyDescent="0.35">
-      <c r="B51" s="4"/>
-      <c r="C51" s="5"/>
-      <c r="D51" s="5"/>
-      <c r="E51" s="13"/>
+      <c r="B51" s="9"/>
+      <c r="C51" s="8"/>
+      <c r="D51" s="8"/>
+      <c r="E51" s="7"/>
     </row>
     <row r="52" spans="2:5" x14ac:dyDescent="0.35">
-      <c r="B52" s="4"/>
-      <c r="C52" s="5"/>
-      <c r="D52" s="5"/>
-      <c r="E52" s="13"/>
-    </row>
-    <row r="57" spans="2:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="60" spans="2:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="72" ht="14.5" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="78" ht="14.5" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="84" ht="14.5" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="90" ht="14.5" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="95" ht="14.5" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="101" ht="14.5" customHeight="1" x14ac:dyDescent="0.35"/>
+      <c r="B52" s="9"/>
+      <c r="C52" s="8"/>
+      <c r="D52" s="8"/>
+      <c r="E52" s="7"/>
+    </row>
+    <row r="53" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B53" s="9"/>
+      <c r="C53" s="8"/>
+      <c r="D53" s="8"/>
+      <c r="E53" s="7"/>
+    </row>
+    <row r="56" spans="2:5" ht="8.5" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="57" spans="2:5" ht="16" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B57" s="17" t="s">
+        <v>30</v>
+      </c>
+      <c r="C57" s="17"/>
+      <c r="D57" s="17"/>
+      <c r="E57" s="17"/>
+    </row>
+    <row r="58" spans="2:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B58" s="17"/>
+      <c r="C58" s="17"/>
+      <c r="D58" s="17"/>
+      <c r="E58" s="17"/>
+    </row>
+    <row r="59" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B59" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C59" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D59" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E59" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="60" spans="2:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B60" s="11" t="s">
+        <v>31</v>
+      </c>
+      <c r="C60" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="D60" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="E60" s="7"/>
+    </row>
+    <row r="61" spans="2:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B61" s="11"/>
+      <c r="C61" s="8"/>
+      <c r="D61" s="8"/>
+      <c r="E61" s="7"/>
+    </row>
+    <row r="62" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B62" s="11"/>
+      <c r="C62" s="8"/>
+      <c r="D62" s="8"/>
+      <c r="E62" s="7"/>
+    </row>
+    <row r="63" spans="2:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B63" s="11"/>
+      <c r="C63" s="8"/>
+      <c r="D63" s="8"/>
+      <c r="E63" s="7"/>
+    </row>
+    <row r="64" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B64" s="11"/>
+      <c r="C64" s="8"/>
+      <c r="D64" s="8"/>
+      <c r="E64" s="7"/>
+    </row>
+    <row r="65" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B65" s="9" t="s">
+        <v>34</v>
+      </c>
+      <c r="C65" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="D65" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="E65" s="7"/>
+    </row>
+    <row r="66" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B66" s="9"/>
+      <c r="C66" s="8"/>
+      <c r="D66" s="8"/>
+      <c r="E66" s="7"/>
+    </row>
+    <row r="67" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B67" s="9"/>
+      <c r="C67" s="8"/>
+      <c r="D67" s="8"/>
+      <c r="E67" s="7"/>
+    </row>
+    <row r="68" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B68" s="9"/>
+      <c r="C68" s="8"/>
+      <c r="D68" s="8"/>
+      <c r="E68" s="7"/>
+    </row>
+    <row r="69" spans="2:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B69" s="9"/>
+      <c r="C69" s="8"/>
+      <c r="D69" s="8"/>
+      <c r="E69" s="7"/>
+    </row>
+    <row r="70" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B70" s="11" t="s">
+        <v>37</v>
+      </c>
+      <c r="C70" s="8" t="s">
+        <v>38</v>
+      </c>
+      <c r="D70" s="8" t="s">
+        <v>39</v>
+      </c>
+      <c r="E70" s="7"/>
+    </row>
+    <row r="71" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B71" s="11"/>
+      <c r="C71" s="8"/>
+      <c r="D71" s="8"/>
+      <c r="E71" s="7"/>
+    </row>
+    <row r="72" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B72" s="11"/>
+      <c r="C72" s="8"/>
+      <c r="D72" s="8"/>
+      <c r="E72" s="7"/>
+    </row>
+    <row r="73" spans="2:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B73" s="11"/>
+      <c r="C73" s="8"/>
+      <c r="D73" s="8"/>
+      <c r="E73" s="7"/>
+    </row>
+    <row r="74" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B74" s="11"/>
+      <c r="C74" s="8"/>
+      <c r="D74" s="8"/>
+      <c r="E74" s="7"/>
+    </row>
+    <row r="75" spans="2:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B75" s="11"/>
+      <c r="C75" s="8" t="s">
+        <v>40</v>
+      </c>
+      <c r="D75" s="8" t="s">
+        <v>41</v>
+      </c>
+      <c r="E75" s="7"/>
+    </row>
+    <row r="76" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B76" s="11"/>
+      <c r="C76" s="8"/>
+      <c r="D76" s="8"/>
+      <c r="E76" s="7"/>
+    </row>
+    <row r="77" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B77" s="11"/>
+      <c r="C77" s="8"/>
+      <c r="D77" s="8"/>
+      <c r="E77" s="7"/>
+    </row>
+    <row r="78" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B78" s="11"/>
+      <c r="C78" s="8"/>
+      <c r="D78" s="8"/>
+      <c r="E78" s="7"/>
+    </row>
+    <row r="79" spans="2:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B79" s="11"/>
+      <c r="C79" s="8"/>
+      <c r="D79" s="8"/>
+      <c r="E79" s="7"/>
+    </row>
+    <row r="80" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B80" s="11"/>
+      <c r="C80" s="8" t="s">
+        <v>42</v>
+      </c>
+      <c r="D80" s="8" t="s">
+        <v>43</v>
+      </c>
+      <c r="E80" s="7"/>
+    </row>
+    <row r="81" spans="2:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B81" s="11"/>
+      <c r="C81" s="8"/>
+      <c r="D81" s="8"/>
+      <c r="E81" s="7"/>
+    </row>
+    <row r="82" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B82" s="11"/>
+      <c r="C82" s="8"/>
+      <c r="D82" s="8"/>
+      <c r="E82" s="7"/>
+    </row>
+    <row r="83" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B83" s="11"/>
+      <c r="C83" s="8"/>
+      <c r="D83" s="8"/>
+      <c r="E83" s="7"/>
+    </row>
+    <row r="84" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B84" s="11"/>
+      <c r="C84" s="8"/>
+      <c r="D84" s="8"/>
+      <c r="E84" s="7"/>
+    </row>
+    <row r="85" spans="2:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="87" spans="2:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="91" spans="2:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="92" spans="2:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="96" spans="2:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="98" ht="14.5" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="102" ht="14.5" customHeight="1" x14ac:dyDescent="0.35"/>
   </sheetData>
-  <mergeCells count="33">
-    <mergeCell ref="E42:E47"/>
-    <mergeCell ref="C48:C52"/>
-    <mergeCell ref="D48:D52"/>
-    <mergeCell ref="E48:E52"/>
-    <mergeCell ref="B31:B52"/>
-    <mergeCell ref="D31:D36"/>
-    <mergeCell ref="E31:E36"/>
-    <mergeCell ref="C37:C41"/>
-    <mergeCell ref="D37:D41"/>
-    <mergeCell ref="E37:E41"/>
-    <mergeCell ref="D19:D24"/>
-    <mergeCell ref="E19:E24"/>
-    <mergeCell ref="C25:C30"/>
-    <mergeCell ref="D25:D30"/>
-    <mergeCell ref="B19:B30"/>
-    <mergeCell ref="E25:E30"/>
-    <mergeCell ref="C19:C24"/>
-    <mergeCell ref="C31:C36"/>
-    <mergeCell ref="G8:H10"/>
-    <mergeCell ref="E7:E12"/>
-    <mergeCell ref="G11:H20"/>
-    <mergeCell ref="C4:C6"/>
-    <mergeCell ref="D4:D6"/>
-    <mergeCell ref="D7:D12"/>
-    <mergeCell ref="C7:C12"/>
-    <mergeCell ref="B4:B18"/>
-    <mergeCell ref="E4:E6"/>
-    <mergeCell ref="B2:E2"/>
-    <mergeCell ref="G2:H2"/>
-    <mergeCell ref="G7:H7"/>
+  <mergeCells count="52">
+    <mergeCell ref="E75:E79"/>
+    <mergeCell ref="C80:C84"/>
+    <mergeCell ref="D80:D84"/>
+    <mergeCell ref="B70:B84"/>
+    <mergeCell ref="E80:E84"/>
+    <mergeCell ref="B65:B69"/>
+    <mergeCell ref="C65:C69"/>
+    <mergeCell ref="D65:D69"/>
+    <mergeCell ref="E65:E69"/>
+    <mergeCell ref="C70:C74"/>
+    <mergeCell ref="D70:D74"/>
+    <mergeCell ref="C75:C79"/>
+    <mergeCell ref="D75:D79"/>
+    <mergeCell ref="B57:E58"/>
+    <mergeCell ref="C60:C64"/>
+    <mergeCell ref="D60:D64"/>
+    <mergeCell ref="B60:B64"/>
+    <mergeCell ref="E60:E64"/>
+    <mergeCell ref="E70:E74"/>
+    <mergeCell ref="B5:B19"/>
+    <mergeCell ref="E5:E7"/>
     <mergeCell ref="G3:H3"/>
-    <mergeCell ref="C42:C47"/>
-    <mergeCell ref="D42:D47"/>
+    <mergeCell ref="G8:H8"/>
+    <mergeCell ref="G4:H4"/>
+    <mergeCell ref="B2:E3"/>
+    <mergeCell ref="G12:H13"/>
+    <mergeCell ref="G9:H11"/>
+    <mergeCell ref="E8:E13"/>
+    <mergeCell ref="C5:C7"/>
+    <mergeCell ref="D5:D7"/>
+    <mergeCell ref="D8:D13"/>
+    <mergeCell ref="C8:C13"/>
+    <mergeCell ref="D20:D25"/>
+    <mergeCell ref="E20:E25"/>
+    <mergeCell ref="C26:C31"/>
+    <mergeCell ref="D26:D31"/>
+    <mergeCell ref="B20:B31"/>
+    <mergeCell ref="E26:E31"/>
+    <mergeCell ref="C20:C25"/>
+    <mergeCell ref="E43:E48"/>
+    <mergeCell ref="C49:C53"/>
+    <mergeCell ref="D49:D53"/>
+    <mergeCell ref="E49:E53"/>
+    <mergeCell ref="B32:B53"/>
+    <mergeCell ref="D32:D37"/>
+    <mergeCell ref="E32:E37"/>
+    <mergeCell ref="C38:C42"/>
+    <mergeCell ref="D38:D42"/>
+    <mergeCell ref="E38:E42"/>
+    <mergeCell ref="C32:C37"/>
+    <mergeCell ref="C43:C48"/>
+    <mergeCell ref="D43:D48"/>
   </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
docs: add mais testes na planilha de teste - SERVICES 1 (#7)
</commit_message>
<xml_diff>
--- a/documentação/planilha-de-teste/planilha-de-teste.xlsx
+++ b/documentação/planilha-de-teste/planilha-de-teste.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="44">
   <si>
     <t>CENÁRIO</t>
   </si>
@@ -176,6 +176,48 @@
   </si>
   <si>
     <t>Dado que eu esteja atualizando usuário associado por ID. Quando eu atualizar e não encontrar por ID. Então deve lançar exceção dizendo que não foi possível encontrar por ID.</t>
+  </si>
+  <si>
+    <t>TESTES API USERS - SERVICES</t>
+  </si>
+  <si>
+    <t>001 - Find All Users</t>
+  </si>
+  <si>
+    <t>CT001-001 - Encontrar todos os usuários deve retornar uma lista Pageable</t>
+  </si>
+  <si>
+    <t>Dado que eu esteja buscando todos os usuários. Quando eu buscar por todos os usuários. Então deve retornar uma lista de usuário Pageable, com tamanho da lista e ordem.</t>
+  </si>
+  <si>
+    <t>002 - Find Users By Username</t>
+  </si>
+  <si>
+    <t>CT002-001 - Encontrar usuários por username deve retornar uma lista de usuários relacionados a aquele nome, mesmo que passe apenas alguns caracteres, por exemplo: "mat"</t>
+  </si>
+  <si>
+    <t>Dado que eu esteja buscando usuário pelo username. Quando eu buscar por username. Então deve retornar uma lista de usuário relacionado a aquele username, com tamanho da página (lista)</t>
+  </si>
+  <si>
+    <t>003 - Find User By Id</t>
+  </si>
+  <si>
+    <t>CT003-001 - Encontrar usuário por ID deve retornar usuário relacionado a aquele ID</t>
+  </si>
+  <si>
+    <t>Dado que eu esteja buscando usuário por ID. Quando eu buscar por ID. Então deve retornar o usuário relacionado a aquele ID.</t>
+  </si>
+  <si>
+    <t>CT003-002 - Caso não encontrar usuário por ID, então deve retonar exceção "No records found for this id!"</t>
+  </si>
+  <si>
+    <t>Dado que eu esteja buscando usuário por ID. Quando eu buscar por ID. Então deve lançar exceção se não encontrar usuário por ID.</t>
+  </si>
+  <si>
+    <t>CT003-002 - Encontrar usuário por ID deve retornar link HATEOAS.</t>
+  </si>
+  <si>
+    <t>Dado que eu esteja buscando usuário por ID. Quando eu buscar por ID. Então deve retornar o usuário e o link HATEOAS.</t>
   </si>
 </sst>
 </file>
@@ -248,7 +290,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="6">
+  <borders count="10">
     <border>
       <left/>
       <right/>
@@ -321,11 +363,55 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -336,18 +422,32 @@
     <xf numFmtId="0" fontId="1" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -357,28 +457,26 @@
     <xf numFmtId="0" fontId="1" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -660,10 +758,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:H101"/>
+  <dimension ref="B2:H102"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="H51" sqref="H51"/>
+    <sheetView tabSelected="1" topLeftCell="A59" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2:E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -676,454 +774,679 @@
     <col min="8" max="8" width="17.81640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:8" ht="18.5" x14ac:dyDescent="0.45">
-      <c r="B2" s="6" t="s">
+    <row r="2" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="B2" s="17" t="s">
         <v>10</v>
       </c>
-      <c r="C2" s="6"/>
-      <c r="D2" s="6"/>
-      <c r="E2" s="6"/>
-      <c r="G2" s="8" t="s">
+      <c r="C2" s="17"/>
+      <c r="D2" s="17"/>
+      <c r="E2" s="17"/>
+    </row>
+    <row r="3" spans="2:8" ht="18.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B3" s="17"/>
+      <c r="C3" s="17"/>
+      <c r="D3" s="17"/>
+      <c r="E3" s="17"/>
+      <c r="G3" s="14" t="s">
         <v>3</v>
       </c>
-      <c r="H2" s="8"/>
-    </row>
-    <row r="3" spans="2:8" x14ac:dyDescent="0.35">
-      <c r="B3" s="1" t="s">
+      <c r="H3" s="14"/>
+    </row>
+    <row r="4" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="B4" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="1" t="s">
+      <c r="C4" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="D3" s="1" t="s">
+      <c r="D4" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="E3" s="1" t="s">
+      <c r="E4" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="G3" s="9" t="s">
+      <c r="G4" s="15" t="s">
         <v>4</v>
       </c>
-      <c r="H3" s="10"/>
-    </row>
-    <row r="4" spans="2:8" x14ac:dyDescent="0.35">
-      <c r="B4" s="15" t="s">
+      <c r="H4" s="16"/>
+    </row>
+    <row r="5" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="B5" s="12" t="s">
         <v>11</v>
       </c>
-      <c r="C4" s="5" t="s">
+      <c r="C5" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="D4" s="5" t="s">
+      <c r="D5" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="E4" s="13"/>
-      <c r="F4" s="11"/>
-      <c r="G4" s="2" t="s">
+      <c r="E5" s="7"/>
+      <c r="F5" s="4"/>
+      <c r="G5" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="H4" s="3"/>
-    </row>
-    <row r="5" spans="2:8" x14ac:dyDescent="0.35">
-      <c r="B5" s="16"/>
-      <c r="C5" s="5"/>
-      <c r="D5" s="5"/>
-      <c r="E5" s="13"/>
-      <c r="G5" s="2" t="s">
+      <c r="H5" s="3"/>
+    </row>
+    <row r="6" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="B6" s="13"/>
+      <c r="C6" s="8"/>
+      <c r="D6" s="8"/>
+      <c r="E6" s="7"/>
+      <c r="G6" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="H5" s="3"/>
-    </row>
-    <row r="6" spans="2:8" x14ac:dyDescent="0.35">
-      <c r="B6" s="16"/>
-      <c r="C6" s="5"/>
-      <c r="D6" s="5"/>
-      <c r="E6" s="13"/>
-    </row>
-    <row r="7" spans="2:8" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B7" s="16"/>
-      <c r="C7" s="5" t="s">
+      <c r="H6" s="3"/>
+    </row>
+    <row r="7" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="B7" s="13"/>
+      <c r="C7" s="8"/>
+      <c r="D7" s="8"/>
+      <c r="E7" s="7"/>
+    </row>
+    <row r="8" spans="2:8" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B8" s="13"/>
+      <c r="C8" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="D7" s="5" t="s">
+      <c r="D8" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="E7" s="13"/>
-      <c r="G7" s="12" t="s">
+      <c r="E8" s="7"/>
+      <c r="G8" s="14" t="s">
         <v>7</v>
       </c>
-      <c r="H7" s="12"/>
-    </row>
-    <row r="8" spans="2:8" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B8" s="16"/>
-      <c r="C8" s="5"/>
-      <c r="D8" s="5"/>
-      <c r="E8" s="13"/>
-      <c r="G8" s="17" t="s">
+      <c r="H8" s="14"/>
+    </row>
+    <row r="9" spans="2:8" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B9" s="13"/>
+      <c r="C9" s="8"/>
+      <c r="D9" s="8"/>
+      <c r="E9" s="7"/>
+      <c r="G9" s="19" t="s">
         <v>8</v>
       </c>
-      <c r="H8" s="17"/>
-    </row>
-    <row r="9" spans="2:8" x14ac:dyDescent="0.35">
-      <c r="B9" s="16"/>
-      <c r="C9" s="5"/>
-      <c r="D9" s="5"/>
-      <c r="E9" s="13"/>
-      <c r="G9" s="17"/>
-      <c r="H9" s="17"/>
+      <c r="H9" s="19"/>
     </row>
     <row r="10" spans="2:8" x14ac:dyDescent="0.35">
-      <c r="B10" s="16"/>
-      <c r="C10" s="5"/>
-      <c r="D10" s="5"/>
-      <c r="E10" s="13"/>
-      <c r="G10" s="17"/>
-      <c r="H10" s="17"/>
-    </row>
-    <row r="11" spans="2:8" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B11" s="16"/>
-      <c r="C11" s="5"/>
-      <c r="D11" s="5"/>
-      <c r="E11" s="13"/>
-      <c r="G11" s="17" t="s">
+      <c r="B10" s="13"/>
+      <c r="C10" s="8"/>
+      <c r="D10" s="8"/>
+      <c r="E10" s="7"/>
+      <c r="G10" s="19"/>
+      <c r="H10" s="19"/>
+    </row>
+    <row r="11" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="B11" s="13"/>
+      <c r="C11" s="8"/>
+      <c r="D11" s="8"/>
+      <c r="E11" s="7"/>
+      <c r="G11" s="19"/>
+      <c r="H11" s="19"/>
+    </row>
+    <row r="12" spans="2:8" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B12" s="13"/>
+      <c r="C12" s="8"/>
+      <c r="D12" s="8"/>
+      <c r="E12" s="7"/>
+      <c r="G12" s="20" t="s">
         <v>9</v>
       </c>
-      <c r="H11" s="17"/>
-    </row>
-    <row r="12" spans="2:8" ht="18" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B12" s="16"/>
-      <c r="C12" s="5"/>
-      <c r="D12" s="5"/>
-      <c r="E12" s="13"/>
-      <c r="G12" s="17"/>
-      <c r="H12" s="17"/>
-    </row>
-    <row r="13" spans="2:8" ht="14.5" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B13" s="16"/>
-      <c r="C13" s="14"/>
-      <c r="D13" s="14"/>
-      <c r="E13" s="14"/>
-      <c r="G13" s="17"/>
-      <c r="H13" s="17"/>
+      <c r="H12" s="21"/>
+    </row>
+    <row r="13" spans="2:8" ht="18" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B13" s="13"/>
+      <c r="C13" s="8"/>
+      <c r="D13" s="8"/>
+      <c r="E13" s="7"/>
+      <c r="G13" s="22"/>
+      <c r="H13" s="23"/>
     </row>
     <row r="14" spans="2:8" ht="14.5" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B14" s="16"/>
-      <c r="C14" s="14"/>
-      <c r="D14" s="14"/>
-      <c r="E14" s="14"/>
-      <c r="G14" s="17"/>
-      <c r="H14" s="17"/>
+      <c r="B14" s="13"/>
+      <c r="C14" s="5"/>
+      <c r="D14" s="5"/>
+      <c r="E14" s="5"/>
+      <c r="G14" s="18"/>
+      <c r="H14" s="18"/>
     </row>
     <row r="15" spans="2:8" ht="14.5" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B15" s="16"/>
-      <c r="C15" s="14"/>
-      <c r="D15" s="14"/>
-      <c r="E15" s="14"/>
-      <c r="G15" s="17"/>
-      <c r="H15" s="17"/>
+      <c r="B15" s="13"/>
+      <c r="C15" s="5"/>
+      <c r="D15" s="5"/>
+      <c r="E15" s="5"/>
+      <c r="G15" s="18"/>
+      <c r="H15" s="18"/>
     </row>
     <row r="16" spans="2:8" ht="14.5" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B16" s="16"/>
-      <c r="C16" s="14"/>
-      <c r="D16" s="14"/>
-      <c r="E16" s="14"/>
-      <c r="G16" s="17"/>
-      <c r="H16" s="17"/>
+      <c r="B16" s="13"/>
+      <c r="C16" s="5"/>
+      <c r="D16" s="5"/>
+      <c r="E16" s="5"/>
+      <c r="G16" s="18"/>
+      <c r="H16" s="18"/>
     </row>
     <row r="17" spans="2:8" ht="14.5" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B17" s="16"/>
-      <c r="C17" s="14"/>
-      <c r="D17" s="14"/>
-      <c r="E17" s="14"/>
-      <c r="G17" s="17"/>
-      <c r="H17" s="17"/>
-    </row>
-    <row r="18" spans="2:8" ht="14.5" hidden="1" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B18" s="16"/>
-      <c r="C18" s="18"/>
-      <c r="D18" s="18"/>
-      <c r="E18" s="18"/>
-      <c r="G18" s="17"/>
-      <c r="H18" s="17"/>
-    </row>
-    <row r="19" spans="2:8" ht="43.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B19" s="7" t="s">
+      <c r="B17" s="13"/>
+      <c r="C17" s="5"/>
+      <c r="D17" s="5"/>
+      <c r="E17" s="5"/>
+      <c r="G17" s="18"/>
+      <c r="H17" s="18"/>
+    </row>
+    <row r="18" spans="2:8" ht="14.5" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B18" s="13"/>
+      <c r="C18" s="5"/>
+      <c r="D18" s="5"/>
+      <c r="E18" s="5"/>
+      <c r="G18" s="18"/>
+      <c r="H18" s="18"/>
+    </row>
+    <row r="19" spans="2:8" ht="14.5" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B19" s="13"/>
+      <c r="C19" s="6"/>
+      <c r="D19" s="6"/>
+      <c r="E19" s="6"/>
+      <c r="G19" s="18"/>
+      <c r="H19" s="18"/>
+    </row>
+    <row r="20" spans="2:8" ht="43.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B20" s="11" t="s">
         <v>16</v>
       </c>
-      <c r="C19" s="5" t="s">
+      <c r="C20" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="D19" s="5" t="s">
+      <c r="D20" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="E19" s="19"/>
-      <c r="G19" s="17"/>
-      <c r="H19" s="17"/>
-    </row>
-    <row r="20" spans="2:8" x14ac:dyDescent="0.35">
-      <c r="B20" s="7"/>
-      <c r="C20" s="5"/>
-      <c r="D20" s="5"/>
-      <c r="E20" s="19"/>
-      <c r="G20" s="17"/>
-      <c r="H20" s="17"/>
+      <c r="E20" s="10"/>
     </row>
     <row r="21" spans="2:8" x14ac:dyDescent="0.35">
-      <c r="B21" s="7"/>
-      <c r="C21" s="5"/>
-      <c r="D21" s="5"/>
-      <c r="E21" s="19"/>
+      <c r="B21" s="11"/>
+      <c r="C21" s="8"/>
+      <c r="D21" s="8"/>
+      <c r="E21" s="10"/>
     </row>
     <row r="22" spans="2:8" x14ac:dyDescent="0.35">
-      <c r="B22" s="7"/>
-      <c r="C22" s="5"/>
-      <c r="D22" s="5"/>
-      <c r="E22" s="19"/>
+      <c r="B22" s="11"/>
+      <c r="C22" s="8"/>
+      <c r="D22" s="8"/>
+      <c r="E22" s="10"/>
     </row>
     <row r="23" spans="2:8" x14ac:dyDescent="0.35">
-      <c r="B23" s="7"/>
-      <c r="C23" s="5"/>
-      <c r="D23" s="5"/>
-      <c r="E23" s="19"/>
+      <c r="B23" s="11"/>
+      <c r="C23" s="8"/>
+      <c r="D23" s="8"/>
+      <c r="E23" s="10"/>
     </row>
     <row r="24" spans="2:8" x14ac:dyDescent="0.35">
-      <c r="B24" s="7"/>
-      <c r="C24" s="5"/>
-      <c r="D24" s="5"/>
-      <c r="E24" s="19"/>
+      <c r="B24" s="11"/>
+      <c r="C24" s="8"/>
+      <c r="D24" s="8"/>
+      <c r="E24" s="10"/>
     </row>
     <row r="25" spans="2:8" x14ac:dyDescent="0.35">
-      <c r="B25" s="7"/>
-      <c r="C25" s="5" t="s">
+      <c r="B25" s="11"/>
+      <c r="C25" s="8"/>
+      <c r="D25" s="8"/>
+      <c r="E25" s="10"/>
+    </row>
+    <row r="26" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="B26" s="11"/>
+      <c r="C26" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="D25" s="5" t="s">
+      <c r="D26" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="E25" s="13"/>
-    </row>
-    <row r="26" spans="2:8" x14ac:dyDescent="0.35">
-      <c r="B26" s="7"/>
-      <c r="C26" s="5"/>
-      <c r="D26" s="5"/>
-      <c r="E26" s="13"/>
+      <c r="E26" s="7"/>
     </row>
     <row r="27" spans="2:8" x14ac:dyDescent="0.35">
-      <c r="B27" s="7"/>
-      <c r="C27" s="5"/>
-      <c r="D27" s="5"/>
-      <c r="E27" s="13"/>
+      <c r="B27" s="11"/>
+      <c r="C27" s="8"/>
+      <c r="D27" s="8"/>
+      <c r="E27" s="7"/>
     </row>
     <row r="28" spans="2:8" x14ac:dyDescent="0.35">
-      <c r="B28" s="7"/>
-      <c r="C28" s="5"/>
-      <c r="D28" s="5"/>
-      <c r="E28" s="13"/>
+      <c r="B28" s="11"/>
+      <c r="C28" s="8"/>
+      <c r="D28" s="8"/>
+      <c r="E28" s="7"/>
     </row>
     <row r="29" spans="2:8" x14ac:dyDescent="0.35">
-      <c r="B29" s="7"/>
-      <c r="C29" s="5"/>
-      <c r="D29" s="5"/>
-      <c r="E29" s="13"/>
+      <c r="B29" s="11"/>
+      <c r="C29" s="8"/>
+      <c r="D29" s="8"/>
+      <c r="E29" s="7"/>
     </row>
     <row r="30" spans="2:8" x14ac:dyDescent="0.35">
-      <c r="B30" s="7"/>
-      <c r="C30" s="5"/>
-      <c r="D30" s="5"/>
-      <c r="E30" s="13"/>
+      <c r="B30" s="11"/>
+      <c r="C30" s="8"/>
+      <c r="D30" s="8"/>
+      <c r="E30" s="7"/>
     </row>
     <row r="31" spans="2:8" x14ac:dyDescent="0.35">
-      <c r="B31" s="4" t="s">
+      <c r="B31" s="11"/>
+      <c r="C31" s="8"/>
+      <c r="D31" s="8"/>
+      <c r="E31" s="7"/>
+    </row>
+    <row r="32" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="B32" s="9" t="s">
         <v>21</v>
       </c>
-      <c r="C31" s="5" t="s">
+      <c r="C32" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="D31" s="5" t="s">
+      <c r="D32" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="E31" s="13"/>
-    </row>
-    <row r="32" spans="2:8" x14ac:dyDescent="0.35">
-      <c r="B32" s="4"/>
-      <c r="C32" s="5"/>
-      <c r="D32" s="5"/>
-      <c r="E32" s="13"/>
+      <c r="E32" s="7"/>
     </row>
     <row r="33" spans="2:5" x14ac:dyDescent="0.35">
-      <c r="B33" s="4"/>
-      <c r="C33" s="5"/>
-      <c r="D33" s="5"/>
-      <c r="E33" s="13"/>
+      <c r="B33" s="9"/>
+      <c r="C33" s="8"/>
+      <c r="D33" s="8"/>
+      <c r="E33" s="7"/>
     </row>
     <row r="34" spans="2:5" x14ac:dyDescent="0.35">
-      <c r="B34" s="4"/>
-      <c r="C34" s="5"/>
-      <c r="D34" s="5"/>
-      <c r="E34" s="13"/>
+      <c r="B34" s="9"/>
+      <c r="C34" s="8"/>
+      <c r="D34" s="8"/>
+      <c r="E34" s="7"/>
     </row>
     <row r="35" spans="2:5" x14ac:dyDescent="0.35">
-      <c r="B35" s="4"/>
-      <c r="C35" s="5"/>
-      <c r="D35" s="5"/>
-      <c r="E35" s="13"/>
+      <c r="B35" s="9"/>
+      <c r="C35" s="8"/>
+      <c r="D35" s="8"/>
+      <c r="E35" s="7"/>
     </row>
     <row r="36" spans="2:5" x14ac:dyDescent="0.35">
-      <c r="B36" s="4"/>
-      <c r="C36" s="5"/>
-      <c r="D36" s="5"/>
-      <c r="E36" s="13"/>
+      <c r="B36" s="9"/>
+      <c r="C36" s="8"/>
+      <c r="D36" s="8"/>
+      <c r="E36" s="7"/>
     </row>
     <row r="37" spans="2:5" x14ac:dyDescent="0.35">
-      <c r="B37" s="4"/>
-      <c r="C37" s="5" t="s">
+      <c r="B37" s="9"/>
+      <c r="C37" s="8"/>
+      <c r="D37" s="8"/>
+      <c r="E37" s="7"/>
+    </row>
+    <row r="38" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B38" s="9"/>
+      <c r="C38" s="8" t="s">
         <v>24</v>
       </c>
-      <c r="D37" s="5" t="s">
+      <c r="D38" s="8" t="s">
         <v>25</v>
       </c>
-      <c r="E37" s="13"/>
-    </row>
-    <row r="38" spans="2:5" x14ac:dyDescent="0.35">
-      <c r="B38" s="4"/>
-      <c r="C38" s="5"/>
-      <c r="D38" s="5"/>
-      <c r="E38" s="13"/>
+      <c r="E38" s="7"/>
     </row>
     <row r="39" spans="2:5" x14ac:dyDescent="0.35">
-      <c r="B39" s="4"/>
-      <c r="C39" s="5"/>
-      <c r="D39" s="5"/>
-      <c r="E39" s="13"/>
+      <c r="B39" s="9"/>
+      <c r="C39" s="8"/>
+      <c r="D39" s="8"/>
+      <c r="E39" s="7"/>
     </row>
     <row r="40" spans="2:5" x14ac:dyDescent="0.35">
-      <c r="B40" s="4"/>
-      <c r="C40" s="5"/>
-      <c r="D40" s="5"/>
-      <c r="E40" s="13"/>
+      <c r="B40" s="9"/>
+      <c r="C40" s="8"/>
+      <c r="D40" s="8"/>
+      <c r="E40" s="7"/>
     </row>
     <row r="41" spans="2:5" x14ac:dyDescent="0.35">
-      <c r="B41" s="4"/>
-      <c r="C41" s="5"/>
-      <c r="D41" s="5"/>
-      <c r="E41" s="13"/>
+      <c r="B41" s="9"/>
+      <c r="C41" s="8"/>
+      <c r="D41" s="8"/>
+      <c r="E41" s="7"/>
     </row>
     <row r="42" spans="2:5" x14ac:dyDescent="0.35">
-      <c r="B42" s="4"/>
-      <c r="C42" s="5" t="s">
+      <c r="B42" s="9"/>
+      <c r="C42" s="8"/>
+      <c r="D42" s="8"/>
+      <c r="E42" s="7"/>
+    </row>
+    <row r="43" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B43" s="9"/>
+      <c r="C43" s="8" t="s">
         <v>26</v>
       </c>
-      <c r="D42" s="5" t="s">
+      <c r="D43" s="8" t="s">
         <v>27</v>
       </c>
-      <c r="E42" s="13"/>
-    </row>
-    <row r="43" spans="2:5" x14ac:dyDescent="0.35">
-      <c r="B43" s="4"/>
-      <c r="C43" s="5"/>
-      <c r="D43" s="5"/>
-      <c r="E43" s="13"/>
+      <c r="E43" s="7"/>
     </row>
     <row r="44" spans="2:5" x14ac:dyDescent="0.35">
-      <c r="B44" s="4"/>
-      <c r="C44" s="5"/>
-      <c r="D44" s="5"/>
-      <c r="E44" s="13"/>
+      <c r="B44" s="9"/>
+      <c r="C44" s="8"/>
+      <c r="D44" s="8"/>
+      <c r="E44" s="7"/>
     </row>
     <row r="45" spans="2:5" x14ac:dyDescent="0.35">
-      <c r="B45" s="4"/>
-      <c r="C45" s="5"/>
-      <c r="D45" s="5"/>
-      <c r="E45" s="13"/>
+      <c r="B45" s="9"/>
+      <c r="C45" s="8"/>
+      <c r="D45" s="8"/>
+      <c r="E45" s="7"/>
     </row>
     <row r="46" spans="2:5" x14ac:dyDescent="0.35">
-      <c r="B46" s="4"/>
-      <c r="C46" s="5"/>
-      <c r="D46" s="5"/>
-      <c r="E46" s="13"/>
+      <c r="B46" s="9"/>
+      <c r="C46" s="8"/>
+      <c r="D46" s="8"/>
+      <c r="E46" s="7"/>
     </row>
     <row r="47" spans="2:5" x14ac:dyDescent="0.35">
-      <c r="B47" s="4"/>
-      <c r="C47" s="5"/>
-      <c r="D47" s="5"/>
-      <c r="E47" s="13"/>
+      <c r="B47" s="9"/>
+      <c r="C47" s="8"/>
+      <c r="D47" s="8"/>
+      <c r="E47" s="7"/>
     </row>
     <row r="48" spans="2:5" x14ac:dyDescent="0.35">
-      <c r="B48" s="4"/>
-      <c r="C48" s="5" t="s">
+      <c r="B48" s="9"/>
+      <c r="C48" s="8"/>
+      <c r="D48" s="8"/>
+      <c r="E48" s="7"/>
+    </row>
+    <row r="49" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B49" s="9"/>
+      <c r="C49" s="8" t="s">
         <v>28</v>
       </c>
-      <c r="D48" s="5" t="s">
+      <c r="D49" s="8" t="s">
         <v>29</v>
       </c>
-      <c r="E48" s="13"/>
-    </row>
-    <row r="49" spans="2:5" x14ac:dyDescent="0.35">
-      <c r="B49" s="4"/>
-      <c r="C49" s="5"/>
-      <c r="D49" s="5"/>
-      <c r="E49" s="13"/>
+      <c r="E49" s="7"/>
     </row>
     <row r="50" spans="2:5" x14ac:dyDescent="0.35">
-      <c r="B50" s="4"/>
-      <c r="C50" s="5"/>
-      <c r="D50" s="5"/>
-      <c r="E50" s="13"/>
+      <c r="B50" s="9"/>
+      <c r="C50" s="8"/>
+      <c r="D50" s="8"/>
+      <c r="E50" s="7"/>
     </row>
     <row r="51" spans="2:5" x14ac:dyDescent="0.35">
-      <c r="B51" s="4"/>
-      <c r="C51" s="5"/>
-      <c r="D51" s="5"/>
-      <c r="E51" s="13"/>
+      <c r="B51" s="9"/>
+      <c r="C51" s="8"/>
+      <c r="D51" s="8"/>
+      <c r="E51" s="7"/>
     </row>
     <row r="52" spans="2:5" x14ac:dyDescent="0.35">
-      <c r="B52" s="4"/>
-      <c r="C52" s="5"/>
-      <c r="D52" s="5"/>
-      <c r="E52" s="13"/>
-    </row>
-    <row r="57" spans="2:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="60" spans="2:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="72" ht="14.5" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="78" ht="14.5" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="84" ht="14.5" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="90" ht="14.5" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="95" ht="14.5" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="101" ht="14.5" customHeight="1" x14ac:dyDescent="0.35"/>
+      <c r="B52" s="9"/>
+      <c r="C52" s="8"/>
+      <c r="D52" s="8"/>
+      <c r="E52" s="7"/>
+    </row>
+    <row r="53" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B53" s="9"/>
+      <c r="C53" s="8"/>
+      <c r="D53" s="8"/>
+      <c r="E53" s="7"/>
+    </row>
+    <row r="56" spans="2:5" ht="8.5" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="57" spans="2:5" ht="16" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B57" s="17" t="s">
+        <v>30</v>
+      </c>
+      <c r="C57" s="17"/>
+      <c r="D57" s="17"/>
+      <c r="E57" s="17"/>
+    </row>
+    <row r="58" spans="2:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B58" s="17"/>
+      <c r="C58" s="17"/>
+      <c r="D58" s="17"/>
+      <c r="E58" s="17"/>
+    </row>
+    <row r="59" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B59" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C59" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D59" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E59" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="60" spans="2:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B60" s="11" t="s">
+        <v>31</v>
+      </c>
+      <c r="C60" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="D60" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="E60" s="7"/>
+    </row>
+    <row r="61" spans="2:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B61" s="11"/>
+      <c r="C61" s="8"/>
+      <c r="D61" s="8"/>
+      <c r="E61" s="7"/>
+    </row>
+    <row r="62" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B62" s="11"/>
+      <c r="C62" s="8"/>
+      <c r="D62" s="8"/>
+      <c r="E62" s="7"/>
+    </row>
+    <row r="63" spans="2:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B63" s="11"/>
+      <c r="C63" s="8"/>
+      <c r="D63" s="8"/>
+      <c r="E63" s="7"/>
+    </row>
+    <row r="64" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B64" s="11"/>
+      <c r="C64" s="8"/>
+      <c r="D64" s="8"/>
+      <c r="E64" s="7"/>
+    </row>
+    <row r="65" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B65" s="9" t="s">
+        <v>34</v>
+      </c>
+      <c r="C65" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="D65" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="E65" s="7"/>
+    </row>
+    <row r="66" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B66" s="9"/>
+      <c r="C66" s="8"/>
+      <c r="D66" s="8"/>
+      <c r="E66" s="7"/>
+    </row>
+    <row r="67" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B67" s="9"/>
+      <c r="C67" s="8"/>
+      <c r="D67" s="8"/>
+      <c r="E67" s="7"/>
+    </row>
+    <row r="68" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B68" s="9"/>
+      <c r="C68" s="8"/>
+      <c r="D68" s="8"/>
+      <c r="E68" s="7"/>
+    </row>
+    <row r="69" spans="2:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B69" s="9"/>
+      <c r="C69" s="8"/>
+      <c r="D69" s="8"/>
+      <c r="E69" s="7"/>
+    </row>
+    <row r="70" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B70" s="11" t="s">
+        <v>37</v>
+      </c>
+      <c r="C70" s="8" t="s">
+        <v>38</v>
+      </c>
+      <c r="D70" s="8" t="s">
+        <v>39</v>
+      </c>
+      <c r="E70" s="7"/>
+    </row>
+    <row r="71" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B71" s="11"/>
+      <c r="C71" s="8"/>
+      <c r="D71" s="8"/>
+      <c r="E71" s="7"/>
+    </row>
+    <row r="72" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B72" s="11"/>
+      <c r="C72" s="8"/>
+      <c r="D72" s="8"/>
+      <c r="E72" s="7"/>
+    </row>
+    <row r="73" spans="2:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B73" s="11"/>
+      <c r="C73" s="8"/>
+      <c r="D73" s="8"/>
+      <c r="E73" s="7"/>
+    </row>
+    <row r="74" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B74" s="11"/>
+      <c r="C74" s="8"/>
+      <c r="D74" s="8"/>
+      <c r="E74" s="7"/>
+    </row>
+    <row r="75" spans="2:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B75" s="11"/>
+      <c r="C75" s="8" t="s">
+        <v>40</v>
+      </c>
+      <c r="D75" s="8" t="s">
+        <v>41</v>
+      </c>
+      <c r="E75" s="7"/>
+    </row>
+    <row r="76" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B76" s="11"/>
+      <c r="C76" s="8"/>
+      <c r="D76" s="8"/>
+      <c r="E76" s="7"/>
+    </row>
+    <row r="77" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B77" s="11"/>
+      <c r="C77" s="8"/>
+      <c r="D77" s="8"/>
+      <c r="E77" s="7"/>
+    </row>
+    <row r="78" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B78" s="11"/>
+      <c r="C78" s="8"/>
+      <c r="D78" s="8"/>
+      <c r="E78" s="7"/>
+    </row>
+    <row r="79" spans="2:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B79" s="11"/>
+      <c r="C79" s="8"/>
+      <c r="D79" s="8"/>
+      <c r="E79" s="7"/>
+    </row>
+    <row r="80" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B80" s="11"/>
+      <c r="C80" s="8" t="s">
+        <v>42</v>
+      </c>
+      <c r="D80" s="8" t="s">
+        <v>43</v>
+      </c>
+      <c r="E80" s="7"/>
+    </row>
+    <row r="81" spans="2:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B81" s="11"/>
+      <c r="C81" s="8"/>
+      <c r="D81" s="8"/>
+      <c r="E81" s="7"/>
+    </row>
+    <row r="82" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B82" s="11"/>
+      <c r="C82" s="8"/>
+      <c r="D82" s="8"/>
+      <c r="E82" s="7"/>
+    </row>
+    <row r="83" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B83" s="11"/>
+      <c r="C83" s="8"/>
+      <c r="D83" s="8"/>
+      <c r="E83" s="7"/>
+    </row>
+    <row r="84" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B84" s="11"/>
+      <c r="C84" s="8"/>
+      <c r="D84" s="8"/>
+      <c r="E84" s="7"/>
+    </row>
+    <row r="85" spans="2:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="87" spans="2:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="91" spans="2:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="92" spans="2:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="96" spans="2:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="98" ht="14.5" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="102" ht="14.5" customHeight="1" x14ac:dyDescent="0.35"/>
   </sheetData>
-  <mergeCells count="33">
-    <mergeCell ref="E42:E47"/>
-    <mergeCell ref="C48:C52"/>
-    <mergeCell ref="D48:D52"/>
-    <mergeCell ref="E48:E52"/>
-    <mergeCell ref="B31:B52"/>
-    <mergeCell ref="D31:D36"/>
-    <mergeCell ref="E31:E36"/>
-    <mergeCell ref="C37:C41"/>
-    <mergeCell ref="D37:D41"/>
-    <mergeCell ref="E37:E41"/>
-    <mergeCell ref="D19:D24"/>
-    <mergeCell ref="E19:E24"/>
-    <mergeCell ref="C25:C30"/>
-    <mergeCell ref="D25:D30"/>
-    <mergeCell ref="B19:B30"/>
-    <mergeCell ref="E25:E30"/>
-    <mergeCell ref="C19:C24"/>
-    <mergeCell ref="C31:C36"/>
-    <mergeCell ref="G8:H10"/>
-    <mergeCell ref="E7:E12"/>
-    <mergeCell ref="G11:H20"/>
-    <mergeCell ref="C4:C6"/>
-    <mergeCell ref="D4:D6"/>
-    <mergeCell ref="D7:D12"/>
-    <mergeCell ref="C7:C12"/>
-    <mergeCell ref="B4:B18"/>
-    <mergeCell ref="E4:E6"/>
-    <mergeCell ref="B2:E2"/>
-    <mergeCell ref="G2:H2"/>
-    <mergeCell ref="G7:H7"/>
+  <mergeCells count="52">
+    <mergeCell ref="E75:E79"/>
+    <mergeCell ref="C80:C84"/>
+    <mergeCell ref="D80:D84"/>
+    <mergeCell ref="B70:B84"/>
+    <mergeCell ref="E80:E84"/>
+    <mergeCell ref="B65:B69"/>
+    <mergeCell ref="C65:C69"/>
+    <mergeCell ref="D65:D69"/>
+    <mergeCell ref="E65:E69"/>
+    <mergeCell ref="C70:C74"/>
+    <mergeCell ref="D70:D74"/>
+    <mergeCell ref="C75:C79"/>
+    <mergeCell ref="D75:D79"/>
+    <mergeCell ref="B57:E58"/>
+    <mergeCell ref="C60:C64"/>
+    <mergeCell ref="D60:D64"/>
+    <mergeCell ref="B60:B64"/>
+    <mergeCell ref="E60:E64"/>
+    <mergeCell ref="E70:E74"/>
+    <mergeCell ref="B5:B19"/>
+    <mergeCell ref="E5:E7"/>
     <mergeCell ref="G3:H3"/>
-    <mergeCell ref="C42:C47"/>
-    <mergeCell ref="D42:D47"/>
+    <mergeCell ref="G8:H8"/>
+    <mergeCell ref="G4:H4"/>
+    <mergeCell ref="B2:E3"/>
+    <mergeCell ref="G12:H13"/>
+    <mergeCell ref="G9:H11"/>
+    <mergeCell ref="E8:E13"/>
+    <mergeCell ref="C5:C7"/>
+    <mergeCell ref="D5:D7"/>
+    <mergeCell ref="D8:D13"/>
+    <mergeCell ref="C8:C13"/>
+    <mergeCell ref="D20:D25"/>
+    <mergeCell ref="E20:E25"/>
+    <mergeCell ref="C26:C31"/>
+    <mergeCell ref="D26:D31"/>
+    <mergeCell ref="B20:B31"/>
+    <mergeCell ref="E26:E31"/>
+    <mergeCell ref="C20:C25"/>
+    <mergeCell ref="E43:E48"/>
+    <mergeCell ref="C49:C53"/>
+    <mergeCell ref="D49:D53"/>
+    <mergeCell ref="E49:E53"/>
+    <mergeCell ref="B32:B53"/>
+    <mergeCell ref="D32:D37"/>
+    <mergeCell ref="E32:E37"/>
+    <mergeCell ref="C38:C42"/>
+    <mergeCell ref="D38:D42"/>
+    <mergeCell ref="E38:E42"/>
+    <mergeCell ref="C32:C37"/>
+    <mergeCell ref="C43:C48"/>
+    <mergeCell ref="D43:D48"/>
   </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>